<commit_message>
work partial for jMapping
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABC56338-7658-4DB6-AC5D-B071FDA3F552}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3F2D0E-B245-473C-9E10-614071A19C72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2535" yWindow="1425" windowWidth="15375" windowHeight="7995" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="128">
   <si>
     <t>ObjReference</t>
   </si>
@@ -372,13 +372,49 @@
   </si>
   <si>
     <t>rentableLease</t>
+  </si>
+  <si>
+    <t>grdAccountNumbers</t>
+  </si>
+  <si>
+    <t>accountTable</t>
+  </si>
+  <si>
+    <t>jeMappingTable</t>
+  </si>
+  <si>
+    <t>grdCashMapping</t>
+  </si>
+  <si>
+    <t>contractType</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='Contract_listbox']</t>
+  </si>
+  <si>
+    <t>//*[@id='Contract_listbox']</t>
+  </si>
+  <si>
+    <t>paymentType</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns='Category_listbox']</t>
+  </si>
+  <si>
+    <t>//*[@id='Category_listbox']</t>
+  </si>
+  <si>
+    <t>gridAccountNumberFilters</t>
+  </si>
+  <si>
+    <t>jMappingAccountTable</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -406,6 +442,12 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF222222"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="3">
@@ -460,7 +502,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -489,6 +531,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1190,7 +1233,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24E92E-F997-460A-B0F8-A599A67DEE36}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1532,15 +1575,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.42578125" customWidth="1"/>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
     <col min="3" max="3" width="38.7109375" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1"/>
@@ -1604,6 +1647,67 @@
         <v>93</v>
       </c>
     </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>120</v>
+      </c>
+      <c r="B8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" t="s">
+        <v>121</v>
+      </c>
+      <c r="D8" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s">
+        <v>124</v>
+      </c>
+      <c r="D9" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" t="s">
+        <v>126</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
create multiple account;create Jmapping
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3F2D0E-B245-473C-9E10-614071A19C72}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{448A0CDA-F479-4C3B-B778-88458EBFA5CD}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="23460" yWindow="4035" windowWidth="15375" windowHeight="7875" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Login" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="128">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="136">
   <si>
     <t>ObjReference</t>
   </si>
@@ -408,6 +408,30 @@
   </si>
   <si>
     <t>jMappingAccountTable</t>
+  </si>
+  <si>
+    <t>//*[@name="cmbChartOfAccount_input"]</t>
+  </si>
+  <si>
+    <t>chartOfAccountInput</t>
+  </si>
+  <si>
+    <t>chartOfAccountList</t>
+  </si>
+  <si>
+    <t>//*[@id="cmbChartOfAccount_listbox"]</t>
+  </si>
+  <si>
+    <t>//*[@aria-controls="cmbChartOfAccount_listbox"]</t>
+  </si>
+  <si>
+    <t>leaseTypes</t>
+  </si>
+  <si>
+    <t>//*[@aria-owns="ddlLeaseTypes_listbox"]</t>
+  </si>
+  <si>
+    <t>//*[@id="ddlLeaseTypes_listbox"]</t>
   </si>
 </sst>
 </file>
@@ -1389,7 +1413,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1575,17 +1599,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="28.42578125" customWidth="1"/>
     <col min="2" max="2" width="37.85546875" customWidth="1"/>
-    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
     <col min="4" max="4" width="42.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1708,6 +1732,45 @@
         <v>126</v>
       </c>
     </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>130</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>132</v>
+      </c>
+      <c r="D12" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>134</v>
+      </c>
+      <c r="D13" t="s">
+        <v>135</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Resolve: marge conflict issues
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,17 +3,18 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11F4B035-EBFB-4D93-848A-C473FF193736}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5D4C4C8-B249-400C-B20E-3931F625B66C}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Login" sheetId="1" r:id="rId1"/>
-    <sheet name="Homepage" sheetId="11" r:id="rId2"/>
-    <sheet name="Property" sheetId="7" r:id="rId3"/>
-    <sheet name="Space" sheetId="10" r:id="rId4"/>
-    <sheet name="Lease" sheetId="8" r:id="rId5"/>
-    <sheet name="GlobalSearch" sheetId="9" r:id="rId6"/>
+    <sheet name="RecurringPayment" sheetId="12" r:id="rId1"/>
+    <sheet name="Login" sheetId="1" r:id="rId2"/>
+    <sheet name="Homepage" sheetId="11" r:id="rId3"/>
+    <sheet name="Property" sheetId="7" r:id="rId4"/>
+    <sheet name="Space" sheetId="10" r:id="rId5"/>
+    <sheet name="Lease" sheetId="8" r:id="rId6"/>
+    <sheet name="GlobalSearch" sheetId="9" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="179">
   <si>
     <t>ObjReference</t>
   </si>
@@ -460,13 +461,115 @@
   </si>
   <si>
     <t>jMappingMaintainCodeType</t>
+  </si>
+  <si>
+    <t>chargeType</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__Charge_listbox')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__Charge-list')]</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__PaymentInfo_listbox')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__PaymentInfo-list')]</t>
+  </si>
+  <si>
+    <t>escalationType</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__EscalationType_listbox')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__EscalationType-list')]</t>
+  </si>
+  <si>
+    <t>leaseTermYear</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__LeaseTermYear_listbox')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__LeaseTermYear-list')]</t>
+  </si>
+  <si>
+    <t>leaseTermDefined</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__LeaseTermDefined_listbox')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__LeaseTermDefined-list')]</t>
+  </si>
+  <si>
+    <t>recurringChargeCurrency</t>
+  </si>
+  <si>
+    <t>//*[contains(@aria-controls,'__Currency_listbox')]</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'__Currency-list')]</t>
+  </si>
+  <si>
+    <t>RecurringCharge_SaveButton</t>
+  </si>
+  <si>
+    <t>RecurringChargeclose</t>
+  </si>
+  <si>
+    <t>btnAddRentalActivity</t>
+  </si>
+  <si>
+    <t>//*[text()='Add Rental Activity']</t>
+  </si>
+  <si>
+    <t>effDate</t>
+  </si>
+  <si>
+    <t>//input[contains(@id,'EFF_DATE')]</t>
+  </si>
+  <si>
+    <t>//input[contains(@id,'END_DATE')]</t>
+  </si>
+  <si>
+    <t>annual</t>
+  </si>
+  <si>
+    <t>//input[contains(@class,'k-formatted-value k-input k-valid')]</t>
+  </si>
+  <si>
+    <t>amount</t>
+  </si>
+  <si>
+    <t>saveRentalActivity</t>
+  </si>
+  <si>
+    <t>//*[text()='Update']</t>
+  </si>
+  <si>
+    <t>addRecurrentPayment</t>
+  </si>
+  <si>
+    <t>//*[text()=' Add New']</t>
+  </si>
+  <si>
+    <t>tableRecurrentPayment</t>
+  </si>
+  <si>
+    <t>grdRentalActivityDetail</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -500,6 +603,13 @@
       <color rgb="FF222222"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -554,7 +664,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -588,11 +698,25 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="12">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -988,6 +1112,240 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
+  <dimension ref="A1:D17"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C24" sqref="C24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="28.42578125" customWidth="1"/>
+    <col min="2" max="2" width="37.85546875" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="42.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" t="s">
+        <v>146</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" t="s">
+        <v>149</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
+        <v>152</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>155</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
+        <v>158</v>
+      </c>
+      <c r="D6" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" t="s">
+        <v>161</v>
+      </c>
+      <c r="D7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="13" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="13" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>166</v>
+      </c>
+      <c r="D10" s="10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="14" t="s">
+        <v>170</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="14" t="s">
+        <v>172</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="14" t="s">
+        <v>173</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="14" t="s">
+        <v>175</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="14" t="s">
+        <v>177</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="10" t="s">
+        <v>178</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="A9:A17">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
@@ -1132,13 +1490,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="11" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E70099-CEBC-4B70-8574-EF45A2018E13}">
   <dimension ref="A1:C2"/>
   <sheetViews>
@@ -1174,34 +1532,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="10" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="9" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="8" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A2">
-    <cfRule type="duplicateValues" dxfId="7" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="6" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="5" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1">
-    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
   <dimension ref="A1:C19"/>
   <sheetViews>
@@ -1427,13 +1785,13 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A8">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC24E92E-F997-460A-B0F8-A599A67DEE36}">
   <dimension ref="A1:D11"/>
   <sheetViews>
@@ -1581,14 +1939,14 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9 A11">
-    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F63B57-EF66-439D-B48A-4F7B8AB73CB4}">
   <dimension ref="A1:D13"/>
   <sheetViews>
@@ -1770,19 +2128,19 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="A9">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
   <dimension ref="A1:D15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Add: 1. TC401TC500 sheet in FASB 2. VerifyCellDataTrue method in UITable 3. isRefreshPageOn method in TestStep Update: MailController.java and PropertyConfig.java
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C8E8E27-4122-4338-82CE-B4AFA969DAB9}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95AA36C-452E-468A-8FEE-809AAA74DA38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="19440" windowHeight="15000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="186">
   <si>
     <t>ObjReference</t>
   </si>
@@ -578,6 +578,12 @@
   </si>
   <si>
     <t>//*[contains(@id,'__SuiteIndex-list')]</t>
+  </si>
+  <si>
+    <t>tbProperty</t>
+  </si>
+  <si>
+    <t>//div[contains(@id,'gridProperty')]</t>
   </si>
 </sst>
 </file>
@@ -1130,7 +1136,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1590,10 +1596,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1810,6 +1816,17 @@
       </c>
       <c r="C19" t="s">
         <v>61</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>184</v>
+      </c>
+      <c r="B20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C20" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add: 1. isPropertyExist method in PropertyCreate.java 2.isLeaseExistWithinProperty method in LeaseCreat.java 3. globalSearch method in UtilKeywordScript.java 4. propertyCode column in lease sheet(DataCreate.xlsx) Update: getSingleRowfromSingleTable method in UITable.java
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F95AA36C-452E-468A-8FEE-809AAA74DA38}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CE3D137-3B09-47A7-83B9-51E69312B964}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="190">
   <si>
     <t>ObjReference</t>
   </si>
@@ -583,7 +583,19 @@
     <t>tbProperty</t>
   </si>
   <si>
-    <t>//div[contains(@id,'gridProperty')]</t>
+    <t>//*[contains(@id,'ddlSearchOptions')]</t>
+  </si>
+  <si>
+    <t>searchOption</t>
+  </si>
+  <si>
+    <t>//div[(@id='gridProperty')]</t>
+  </si>
+  <si>
+    <t>tbLease</t>
+  </si>
+  <si>
+    <t>//div[(@id='id_376368_C_ctl01_ucPSPC_gvPropertyContracts')]</t>
   </si>
 </sst>
 </file>
@@ -1596,10 +1608,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
-  <dimension ref="A1:C20"/>
+  <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1826,7 +1838,18 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>185</v>
+        <v>187</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>188</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
+        <v>189</v>
       </c>
     </row>
   </sheetData>
@@ -2194,10 +2217,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2246,151 +2269,163 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>186</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>92</v>
-      </c>
+        <v>185</v>
+      </c>
+      <c r="D4" s="10"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>113</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>116</v>
+        <v>93</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="10" t="s">
-        <v>119</v>
+      <c r="C7" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>121</v>
-      </c>
-      <c r="D8" t="s">
-        <v>122</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="10" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D9" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>126</v>
+        <v>124</v>
+      </c>
+      <c r="D10" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>132</v>
-      </c>
-      <c r="D12" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>139</v>
+        <v>133</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="D14" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>139</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>140</v>
+      </c>
+      <c r="D15" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>144</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>142</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>143</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: 1. isLeaseExist method 2. globalSearch method Add: 1. isSpaceExistWithenProperty and isRecurringPaymentExist in leaseCreate.java 2. navigateToProperty in propertyCrteate.java 3. add UIPanel.java 4. verifyCorrespondingDataTrue in UITable.java
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CF0C6E2-F35C-485E-B429-892950E186E2}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613802F4-04ED-42AD-9433-F89FF0A55753}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="12" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="298" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="195">
   <si>
     <t>ObjReference</t>
   </si>
@@ -587,6 +587,30 @@
   </si>
   <si>
     <t>//div[(@id='id_376368_C_ctl01_ucPSPC_gvPropertyContracts')]</t>
+  </si>
+  <si>
+    <t>searchOption</t>
+  </si>
+  <si>
+    <t>//*[contains(@id,'ddlSearchOptions')]</t>
+  </si>
+  <si>
+    <t>tbRPayment</t>
+  </si>
+  <si>
+    <t>//div[contains(@id,"grdRecurringPaymentsReceivables_")]/div[2]/div</t>
+  </si>
+  <si>
+    <t>link</t>
+  </si>
+  <si>
+    <t>//*[@class='expandAll']</t>
+  </si>
+  <si>
+    <t>tbSpace</t>
+  </si>
+  <si>
+    <t>//div[(@id='id_376367_C_ctl01_ucPSS_gvSuites_GridData')]</t>
   </si>
 </sst>
 </file>
@@ -688,7 +712,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -720,7 +744,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1134,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1382,7 +1405,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
@@ -1589,10 +1612,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+      <selection activeCell="A25" sqref="A25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1823,14 +1846,25 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" t="s">
         <v>185</v>
       </c>
-      <c r="B21" s="13" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="13" t="s">
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
         <v>186</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>193</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
+        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -1998,17 +2032,17 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96F63B57-EF66-439D-B48A-4F7B8AB73CB4}">
-  <dimension ref="A1:D14"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.28515625" customWidth="1"/>
     <col min="2" max="2" width="19.5703125" customWidth="1"/>
-    <col min="3" max="3" width="57.140625" customWidth="1"/>
+    <col min="3" max="3" width="64.7109375" customWidth="1"/>
     <col min="4" max="4" width="56.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2185,6 +2219,28 @@
       </c>
       <c r="C14" t="s">
         <v>175</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>189</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>191</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2198,10 +2254,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D5E6D20C-25AD-4167-A7E6-F426B5200648}">
-  <dimension ref="A1:D15"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="C27" sqref="C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2250,151 +2306,163 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>8</v>
+        <v>187</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>88</v>
-      </c>
+        <v>188</v>
+      </c>
+      <c r="D4" s="9"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>109</v>
+        <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="B6" t="s">
         <v>10</v>
       </c>
       <c r="C6" t="s">
-        <v>112</v>
+        <v>89</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="9" t="s">
-        <v>115</v>
+      <c r="C7" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" t="s">
-        <v>117</v>
-      </c>
-      <c r="D8" t="s">
-        <v>118</v>
+        <v>10</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>115</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B9" t="s">
         <v>11</v>
       </c>
       <c r="C9" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="D9" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" t="s">
-        <v>122</v>
+        <v>120</v>
+      </c>
+      <c r="D10" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B12" t="s">
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>128</v>
-      </c>
-      <c r="D12" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="D13" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
       </c>
       <c r="C14" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="D14" t="s">
-        <v>136</v>
+        <v>131</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>134</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>135</v>
+      </c>
+      <c r="D15" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>139</v>
       </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>137</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D16" t="s">
         <v>138</v>
       </c>
     </row>

</xml_diff>

<commit_message>
partial commit for revision post
</commit_message>
<xml_diff>
--- a/src/main/resources/objectLocator/Common.xlsx
+++ b/src/main/resources/objectLocator/Common.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{613802F4-04ED-42AD-9433-F89FF0A55753}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6F3F2E6-8FEE-4EDD-A4C0-16390A250FBA}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="330" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RecurringPayment" sheetId="12" r:id="rId1"/>
@@ -568,9 +568,6 @@
     <t>tbProperty</t>
   </si>
   <si>
-    <t>//div[contains(@id,'gridProperty')]</t>
-  </si>
-  <si>
     <t>propertyGroup1</t>
   </si>
   <si>
@@ -611,6 +608,9 @@
   </si>
   <si>
     <t>//div[(@id='id_376367_C_ctl01_ucPSS_gvSuites_GridData')]</t>
+  </si>
+  <si>
+    <t>//div[@id='gridProperty']</t>
   </si>
 </sst>
 </file>
@@ -1157,7 +1157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CD51E865-2458-4A55-AA79-2C102593FD0A}">
   <dimension ref="A1:D18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -1614,8 +1614,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C63457F8-4820-4E80-A0BD-86B1DB623BD5}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A25" sqref="A25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1759,7 +1759,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B13" t="s">
         <v>11</v>
@@ -1770,7 +1770,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B14" t="s">
         <v>11</v>
@@ -1781,7 +1781,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B15" t="s">
         <v>11</v>
@@ -1842,29 +1842,29 @@
         <v>11</v>
       </c>
       <c r="C20" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>184</v>
+      </c>
+      <c r="B21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" t="s">
         <v>185</v>
-      </c>
-      <c r="B21" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>192</v>
+      </c>
+      <c r="B22" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" t="s">
         <v>193</v>
-      </c>
-      <c r="B22" t="s">
-        <v>11</v>
-      </c>
-      <c r="C22" t="s">
-        <v>194</v>
       </c>
     </row>
   </sheetData>
@@ -2176,7 +2176,7 @@
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
@@ -2223,24 +2223,24 @@
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>188</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
         <v>189</v>
-      </c>
-      <c r="B15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
+        <v>190</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
         <v>191</v>
-      </c>
-      <c r="B16" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" t="s">
-        <v>192</v>
       </c>
     </row>
   </sheetData>
@@ -2306,13 +2306,13 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>186</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" t="s">
         <v>187</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>188</v>
       </c>
       <c r="D4" s="9"/>
     </row>

</xml_diff>